<commit_message>
initial version for Laura
</commit_message>
<xml_diff>
--- a/data/baltic_geochem.xlsx
+++ b/data/baltic_geochem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewsteen/Dropbox (Personal)/misc/baltic_CH4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FDAD7D6-7C22-1E48-B451-A12A38980500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F3DDE9-DD08-F74B-AC86-C9DE4CA65149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-620" yWindow="6460" windowWidth="28800" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7625,7 +7625,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I101" sqref="I101"/>
+      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -11840,6 +11840,9 @@
       <c r="H101" s="2">
         <v>6.5</v>
       </c>
+      <c r="I101" s="2">
+        <v>9.4</v>
+      </c>
       <c r="L101" s="42">
         <v>3.056</v>
       </c>
@@ -11877,6 +11880,9 @@
       </c>
       <c r="H102" s="2">
         <v>5.4</v>
+      </c>
+      <c r="I102" s="2">
+        <v>1.8</v>
       </c>
       <c r="L102" s="42">
         <v>4.8</v>

</xml_diff>